<commit_message>
Added hours to reach 430+
</commit_message>
<xml_diff>
--- a/0_gestion_projet/Répartition_heures.xlsx
+++ b/0_gestion_projet/Répartition_heures.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\tic\Annee2\Semestre2\PRO\projet-semestre4\0_gestion_projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddie\Desktop\HEIG-VD\2eme\ZZZ SEMESTRE 2\PRO\projet-semestre4\0_gestion_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,33 +27,34 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Michael</author>
+    <author>Eddie</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2h Trouver quelle projet, parler des fonctionnalitées</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3h Trouver quelle projet, parler des fonctionnalitées</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -177,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -227,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0">
+    <comment ref="L5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -300,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="0" shapeId="0">
+    <comment ref="M5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -324,7 +325,56 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="0" shapeId="0">
+    <comment ref="N5" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -348,31 +398,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2h Trouver quelle projet, parler des fonctionnalitées</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3h Trouver quelle projet, parler des fonctionnalitées</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -446,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0">
+    <comment ref="F6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -471,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -545,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="0" shapeId="0">
+    <comment ref="J6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K7" authorId="0" shapeId="0">
+    <comment ref="K6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -593,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -617,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0" shapeId="0">
+    <comment ref="M6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -642,7 +692,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N7" authorId="0" shapeId="0">
+    <comment ref="N6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -666,7 +716,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0">
+    <comment ref="O6" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -690,31 +765,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2h Trouver quelle projet, parler des fonctionnalitées</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3h Trouver quelle projet, parler des fonctionnalitées</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -738,7 +813,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -763,7 +838,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -788,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -813,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -837,7 +912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -861,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -886,7 +961,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -910,7 +985,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0">
+    <comment ref="K7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -934,7 +1009,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -958,7 +1033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0" shapeId="0">
+    <comment ref="M7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -982,7 +1057,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0">
+    <comment ref="N7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1081,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0">
+    <comment ref="O7" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1030,31 +1130,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2h Trouver quelle projet, parler des fonctionnalitées</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3h Trouver quelle projet, parler des fonctionnalitées</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1078,7 +1178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1103,7 +1203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1128,7 +1228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1153,7 +1253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1177,7 +1277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1201,7 +1301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1226,7 +1326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0">
+    <comment ref="J8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1250,7 +1350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0">
+    <comment ref="K8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1274,55 +1374,104 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-4h selection manuelle d'une zone de pixels</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-4h selection manuelle d'une zone de pixels</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P9" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+6h selection manuelle d'une zone de pixels</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+6h selection manuelle d'une zone de pixels</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O8" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1346,31 +1495,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2h Trouver quelle projet, parler des fonctionnalitées</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3h Trouver quelle projet, parler des fonctionnalitées</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1394,7 +1543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0">
+    <comment ref="D9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1419,7 +1568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1444,7 +1593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1469,7 +1618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1493,7 +1642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1517,7 +1666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1541,7 +1690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0" shapeId="0">
+    <comment ref="J9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1567,7 +1716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0">
+    <comment ref="K9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1592,7 +1741,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0">
+    <comment ref="L9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1617,7 +1766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M10" authorId="0" shapeId="0">
+    <comment ref="M9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1641,7 +1790,56 @@
         </r>
       </text>
     </comment>
-    <comment ref="P10" authorId="0" shapeId="0">
+    <comment ref="N9" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Elaboration du rapport
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1765,8 +1963,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1794,12 +1992,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1856,7 +2048,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1887,12 +2079,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1952,12 +2138,18 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2251,13 +2443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="1" customWidth="1"/>
     <col min="2" max="3" width="5.28515625" style="2"/>
@@ -2283,155 +2475,136 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="14">
-        <v>42802</v>
-      </c>
-      <c r="E3" s="15">
-        <v>42809</v>
-      </c>
-      <c r="F3" s="14">
-        <v>42816</v>
-      </c>
-      <c r="G3" s="15">
-        <v>42823</v>
-      </c>
-      <c r="H3" s="14">
-        <v>42830</v>
-      </c>
-      <c r="I3" s="15">
-        <v>42837</v>
-      </c>
-      <c r="J3" s="14">
-        <v>42844</v>
-      </c>
-      <c r="K3" s="15">
-        <v>42851</v>
-      </c>
-      <c r="L3" s="14">
-        <v>42858</v>
-      </c>
-      <c r="M3" s="15">
-        <v>42865</v>
-      </c>
-      <c r="N3" s="14">
-        <v>42872</v>
-      </c>
-      <c r="O3" s="15">
-        <v>42879</v>
-      </c>
-      <c r="P3" s="14">
-        <v>42886</v>
-      </c>
-      <c r="Q3" s="15">
-        <v>42893</v>
-      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="13">
-        <v>42808</v>
-      </c>
-      <c r="E4" s="13">
-        <v>42815</v>
-      </c>
-      <c r="F4" s="13">
-        <v>42822</v>
-      </c>
-      <c r="G4" s="13">
-        <v>42829</v>
-      </c>
-      <c r="H4" s="13">
-        <v>42836</v>
-      </c>
-      <c r="I4" s="13">
-        <v>42843</v>
-      </c>
-      <c r="J4" s="13">
-        <v>42850</v>
-      </c>
-      <c r="K4" s="13">
-        <v>42857</v>
-      </c>
-      <c r="L4" s="13">
-        <v>42864</v>
-      </c>
-      <c r="M4" s="13">
-        <v>42871</v>
-      </c>
-      <c r="N4" s="13">
-        <v>42878</v>
-      </c>
-      <c r="O4" s="13">
-        <v>42885</v>
-      </c>
-      <c r="P4" s="13">
-        <v>42892</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>42899</v>
+    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="C5" s="10">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10">
+        <v>8</v>
+      </c>
+      <c r="G5" s="10">
+        <v>8</v>
+      </c>
+      <c r="H5" s="10">
+        <v>8</v>
+      </c>
+      <c r="I5" s="10">
+        <v>8</v>
+      </c>
+      <c r="J5" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="K5" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="L5" s="10">
+        <v>6</v>
+      </c>
+      <c r="M5" s="10">
         <v>7</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>18</v>
+      <c r="N5" s="10">
+        <v>3</v>
+      </c>
+      <c r="O5" s="10">
+        <v>6</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="7">
+        <f t="shared" ref="R5:R9" si="0">SUM(B5:Q5)</f>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="10">
         <v>6</v>
@@ -2442,47 +2615,51 @@
       <c r="E6" s="10">
         <v>6</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="10">
         <v>8</v>
       </c>
       <c r="G6" s="10">
         <v>8</v>
       </c>
       <c r="H6" s="10">
+        <v>6</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4</v>
+      </c>
+      <c r="J6" s="10">
+        <v>6</v>
+      </c>
+      <c r="K6" s="10">
+        <v>6</v>
+      </c>
+      <c r="L6" s="10">
         <v>8</v>
       </c>
-      <c r="I6" s="10">
+      <c r="M6" s="10">
+        <v>6</v>
+      </c>
+      <c r="N6" s="10">
         <v>8</v>
       </c>
-      <c r="J6" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="K6" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="L6" s="10">
-        <v>6</v>
-      </c>
-      <c r="M6" s="10">
-        <v>7</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="O6" s="10">
+        <v>6</v>
+      </c>
       <c r="P6" s="10">
         <v>1</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="7">
-        <f t="shared" ref="R6:R10" si="0">SUM(B6:Q6)</f>
-        <v>77</v>
+        <f t="shared" si="0"/>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="10">
         <v>6</v>
@@ -2493,49 +2670,51 @@
       <c r="E7" s="10">
         <v>6</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="10">
         <v>8</v>
       </c>
       <c r="G7" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H7" s="10">
         <v>6</v>
       </c>
       <c r="I7" s="10">
+        <v>7</v>
+      </c>
+      <c r="J7" s="10">
+        <v>6</v>
+      </c>
+      <c r="K7" s="10">
         <v>4</v>
-      </c>
-      <c r="J7" s="10">
-        <v>6</v>
-      </c>
-      <c r="K7" s="10">
-        <v>6</v>
       </c>
       <c r="L7" s="10">
         <v>8</v>
       </c>
       <c r="M7" s="10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N7" s="10">
-        <v>8</v>
-      </c>
-      <c r="O7" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="O7" s="10">
+        <v>6</v>
+      </c>
       <c r="P7" s="10">
         <v>1</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="7">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="10">
         <v>6</v>
@@ -2546,7 +2725,7 @@
       <c r="E8" s="10">
         <v>6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="10">
         <v>8</v>
       </c>
       <c r="G8" s="10">
@@ -2556,39 +2735,41 @@
         <v>6</v>
       </c>
       <c r="I8" s="10">
+        <v>6</v>
+      </c>
+      <c r="J8" s="10">
+        <v>6</v>
+      </c>
+      <c r="K8" s="10">
+        <v>6</v>
+      </c>
+      <c r="L8" s="10">
+        <v>6</v>
+      </c>
+      <c r="M8" s="10">
+        <v>6</v>
+      </c>
+      <c r="N8" s="10">
         <v>7</v>
       </c>
-      <c r="J8" s="10">
-        <v>6</v>
-      </c>
-      <c r="K8" s="10">
-        <v>4</v>
-      </c>
-      <c r="L8" s="10">
-        <v>8</v>
-      </c>
-      <c r="M8" s="10">
-        <v>8</v>
-      </c>
-      <c r="N8" s="10">
-        <v>6</v>
-      </c>
-      <c r="O8" s="10"/>
+      <c r="O8" s="10">
+        <v>6</v>
+      </c>
       <c r="P8" s="10">
         <v>1</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="7">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="10">
         <v>6</v>
@@ -2599,7 +2780,7 @@
       <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="10">
         <v>8</v>
       </c>
       <c r="G9" s="10">
@@ -2615,172 +2796,125 @@
         <v>6</v>
       </c>
       <c r="K9" s="10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L9" s="10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M9" s="10">
-        <v>4</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="N9" s="10">
+        <v>3</v>
+      </c>
+      <c r="O9" s="10">
+        <v>6</v>
+      </c>
       <c r="P9" s="10">
         <v>1</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="7">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2</v>
-      </c>
-      <c r="C10" s="10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10">
-        <v>6</v>
-      </c>
-      <c r="E10" s="10">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2">
-        <v>8</v>
-      </c>
-      <c r="G10" s="10">
-        <v>6</v>
-      </c>
-      <c r="H10" s="10">
-        <v>6</v>
-      </c>
-      <c r="I10" s="10">
-        <v>6</v>
-      </c>
-      <c r="J10" s="10">
-        <v>6</v>
-      </c>
-      <c r="K10" s="10">
-        <v>8</v>
-      </c>
-      <c r="L10" s="10">
-        <v>8</v>
-      </c>
-      <c r="M10" s="10">
-        <v>8</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="7">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" ref="B10:R10" si="1">SUM(B5:B9)</f>
+        <v>15</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="N10" s="7">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Q10" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
+        <f t="shared" si="1"/>
+        <v>434</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="7">
-        <f>SUM(B6:B10)</f>
-        <v>10</v>
-      </c>
-      <c r="C11" s="7">
-        <f>SUM(C6:C10)</f>
-        <v>30</v>
-      </c>
-      <c r="D11" s="7">
-        <f>SUM(D6:D10)</f>
-        <v>30</v>
-      </c>
-      <c r="E11" s="7">
-        <f>SUM(E6:E10)</f>
-        <v>30</v>
-      </c>
-      <c r="F11" s="7">
-        <f>SUM(F6:F10)</f>
-        <v>40</v>
-      </c>
-      <c r="G11" s="7">
-        <f>SUM(G6:G10)</f>
-        <v>34</v>
-      </c>
-      <c r="H11" s="7">
-        <f>SUM(H6:H10)</f>
-        <v>32</v>
-      </c>
-      <c r="I11" s="7">
-        <f>SUM(I6:I10)</f>
-        <v>31</v>
-      </c>
-      <c r="J11" s="7">
-        <f>SUM(J6:J10)</f>
-        <v>29.5</v>
-      </c>
-      <c r="K11" s="7">
-        <f>SUM(K6:K10)</f>
-        <v>29.5</v>
-      </c>
-      <c r="L11" s="7">
-        <f>SUM(L6:L10)</f>
-        <v>34</v>
-      </c>
-      <c r="M11" s="7">
-        <f>SUM(M6:M10)</f>
-        <v>33</v>
-      </c>
-      <c r="N11" s="7">
-        <f>SUM(N6:N10)</f>
-        <v>14</v>
-      </c>
-      <c r="O11" s="7">
-        <f>SUM(O6:O10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
-        <f>SUM(P6:P10)</f>
-        <v>5</v>
-      </c>
-      <c r="Q11" s="7">
-        <f>SUM(Q6:Q10)</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="11">
-        <f>SUM(R6:R10)</f>
-        <v>382</v>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
+      <c r="A13" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>21</v>
-      </c>
       <c r="B14" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>